<commit_message>
Sparql normalizer (cat 0), bug fixes (#34)
* new queries

* fix docu

* tmp old tests

* fix spelling

* tmp old tests

* update ALLOWED HOSTS

* add

* fix bug

* bug fixes, normalize_sparql

* test for Normalize.normalize_sparql

* initial

* remove old tests
</commit_message>
<xml_diff>
--- a/django/bartocgraphql/fixtures/sparqlendpoints.xlsx
+++ b/django/bartocgraphql/fixtures/sparqlendpoints.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14130"/>
   </bookViews>
   <sheets>
     <sheet name="LuSTRE" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>name</t>
   </si>
@@ -45,12 +45,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>Return subjects whose skos:definition contains searchword</t>
-  </si>
-  <si>
-    <t>Return subjects whose rdfs:label contains searchword</t>
-  </si>
-  <si>
     <t>http://vocab.getty.edu/sparql</t>
   </si>
   <si>
@@ -67,22 +61,6 @@
   </si>
   <si>
     <t>Getty</t>
-  </si>
-  <si>
-    <t>SELECT distinct ?subject ?predicate ?object
-WHERE {
-  ?subject rdfs:label ?object .
-  ?subject ?predicate ?object .
-  FILTER regex(?object, "!!!SEARCHWORD!!!" , "i")
-}</t>
-  </si>
-  <si>
-    <t>SELECT distinct ?subject ?predicate ?object
-WHERE {
-  ?subject skos:definition ?object .
-  ?subject ?predicate ?object .
-  FILTER regex(?object, "!!!SEARCHWORD!!!", "i")
-}</t>
   </si>
   <si>
     <t>http://vocab.getty.edu/queries#Combination_Full-Text_and_Exact_String_Match</t>
@@ -100,22 +78,76 @@
         optional {?Subject skos:scopeNote [dct:language gvp_lang:en; rdf:value ?ScopeNote]}}</t>
   </si>
   <si>
+    <t>timeout</t>
+  </si>
+  <si>
     <t>select ?x ?label {
         ?x luc:term "!!!SEARCHWORD!!!";
         gvp:prefLabelGVP/xl:literalForm ?label.
         filter exists {
         ?x (xl:prefLabel|xl:altLabel)/gvp:term ?term.
-        filter (lcase(str(?term))="!!!SEARCHWORD!!!" &amp;&amp; langMatches(lang(?term),"en"))}}</t>
-  </si>
-  <si>
-    <t>timeout</t>
+        filter (lcase(str(?term))="!!!SEARCHWORD!!!" &amp;&amp; langMatches(lang(?term),"en"))}}
+LIMIT 100</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?subject ?predicate ?object
+WHERE {
+  ?subject skos:definition ?object .
+  ?subject ?predicate ?object .
+  FILTER regex(?object, "!!!SEARCHWORD!!!", "i")
+}</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?subject ?predicate ?object
+WHERE {
+  ?subject rdfs:label ?object .
+  ?subject ?predicate ?object .
+  FILTER regex(?object, "!!!SEARCHWORD!!!" , "i")
+} 
+LIMIT 100</t>
+  </si>
+  <si>
+    <t>Return subjects whose skos:definition contains searchword.</t>
+  </si>
+  <si>
+    <t>Return subjects whose rdfs:label contains searchword; limited to 100.</t>
+  </si>
+  <si>
+    <t>Return subjects whose rdfs:label bif:contains searchword; ordered by score and limited to 100.
+# http://www.openlinksw.com/schemas/bif# is a feature of SPARQL Virtuoso server, see http://docs.openlinksw.com/virtuoso/rdfsparqlrulefulltext/
+# could be made more permissive with wildcard " ' !!!SEARCHWORD!!! * ' " but also much slower</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?subject ?predicate ?object
+WHERE {
+  ?subject rdfs:label ?object .
+  ?subject luc:term "!!!SEARCHWORD!!!" .
+  ?subject ?predicate ?object .
+  FILTER regex(?object, "!!!SEARCHWORD!!!" , "i")
+} 
+LIMIT 100</t>
+  </si>
+  <si>
+    <t>Return subjects whose rdfs:label contains searchword; limited to 100.
+# http://www.ontotext.com/owlim/lucene# Ontotext GraphDB's built-in Lucene Full Text Search, see http://vocab.getty.edu/doc/#Full_Text_Search</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT ?subject ?predicate ?object
+WHERE {
+  ?subject rdfs:label ?object .
+  ?subject ?predicate ?object .
+  ?object bif:contains "!!!SEARCHWORD!!!" 
+  OPTION (score ?sc) .
+} 
+ORDER BY DESC (?sc)
+LIMIT 100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +171,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -157,18 +197,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,32 +506,32 @@
     <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -496,31 +539,46 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
+        <v>16</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>222</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
+    </row>
+    <row r="5" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -530,10 +588,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="46.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +609,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -559,49 +617,63 @@
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
+      <c r="D3" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>222</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="C4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>0</v>
       </c>
     </row>

</xml_diff>